<commit_message>
Tabla de datos con estilo con bandas
</commit_message>
<xml_diff>
--- a/02/TablaDatos.xlsx
+++ b/02/TablaDatos.xlsx
@@ -879,6 +879,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla1" displayName="Tabla1" ref="A2:I231" totalsRowShown="0">
+  <autoFilter ref="A2:I231"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Continente"/>
+    <tableColumn id="2" name="País"/>
+    <tableColumn id="3" name="Hombres"/>
+    <tableColumn id="4" name="Mujeres"/>
+    <tableColumn id="5" name="% P. femenina">
+      <calculatedColumnFormula>+D3/(C3+D3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Rural"/>
+    <tableColumn id="7" name="Urbana"/>
+    <tableColumn id="8" name="Total país"/>
+    <tableColumn id="9" name="% P. rural">
+      <calculatedColumnFormula>+F3/(F3+G3)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8589,5 +8611,8 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tabla de datos con segmentación
</commit_message>
<xml_diff>
--- a/02/TablaDatos.xlsx
+++ b/02/TablaDatos.xlsx
@@ -14,8 +14,19 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="SegmentaciónDeDatos_Continente">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
+      <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicerCache r:id="rId2"/>
+      </x15:slicerCaches>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -881,9 +892,108 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Continente"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Continente"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7115175" y="2314576"/>
+              <a:ext cx="2457450" cy="2019300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos de tabla. La segmentación de datos de tabla se admite en Excel o versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2007 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Continente" sourceName="Continente">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="3" column="1"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Continente" cache="SegmentaciónDeDatos_Continente" caption="Continente" columnCount="2" style="SlicerStyleLight4" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla1" displayName="Tabla1" ref="A2:I231" totalsRowShown="0">
-  <autoFilter ref="A2:I231"/>
+  <autoFilter ref="A2:I231">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Europa"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="9">
     <tableColumn id="1" name="Continente"/>
     <tableColumn id="2" name="País"/>
@@ -1225,7 +1335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1257,7 +1367,7 @@
         <v>0.56937904447198129</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1289,7 +1399,7 @@
         <v>0.54321924226873131</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1321,7 +1431,7 @@
         <v>0.82821834847368847</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1353,7 +1463,7 @@
         <v>0.70038740439058311</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1385,7 +1495,7 @@
         <v>0.49854636591478696</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1527,7 @@
         <v>0.72926323493535006</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1449,7 +1559,7 @@
         <v>0.41473321635146554</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1481,7 +1591,7 @@
         <v>0.67853396054011983</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1513,7 +1623,7 @@
         <v>0.64889381296956683</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1545,7 +1655,7 @@
         <v>0.45390605375533788</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1577,7 +1687,7 @@
         <v>0.86179823109303311</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1609,7 +1719,7 @@
         <v>0.62150625063522713</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1641,7 +1751,7 @@
         <v>0.61142797884475786</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1673,7 +1783,7 @@
         <v>0.71140939597315433</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1705,7 +1815,7 @@
         <v>0.51949908119512689</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1737,7 +1847,7 @@
         <v>0.5410987195373812</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1769,7 +1879,7 @@
         <v>0.66476999519153712</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1801,7 +1911,7 @@
         <v>0.82085055096418735</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1833,7 +1943,7 @@
         <v>0.65426316245988381</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1865,7 +1975,7 @@
         <v>0.70629562043795624</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1897,7 +2007,7 @@
         <v>0.85048397706982426</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1929,7 +2039,7 @@
         <v>0.7993269230769231</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1961,7 +2071,7 @@
         <v>0.72890818858560791</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1993,7 +2103,7 @@
         <v>0.35211416490486258</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2025,7 +2135,7 @@
         <v>0.53685463794782984</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2057,7 +2167,7 @@
         <v>0.5577094474153298</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2089,7 +2199,7 @@
         <v>0.76535264145883619</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2121,7 +2231,7 @@
         <v>0.67971191738007886</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2153,7 +2263,7 @@
         <v>0.93946095369730476</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2185,7 +2295,7 @@
         <v>0.91348057882711353</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2217,7 +2327,7 @@
         <v>0.58531244736398857</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2249,7 +2359,7 @@
         <v>0.12831292268323891</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2281,7 +2391,7 @@
         <v>0.64066143735425063</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2313,7 +2423,7 @@
         <v>0.67250166186572125</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2345,7 +2455,7 @@
         <v>0.81607959128798069</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2377,7 +2487,7 @@
         <v>0.59239436619718311</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2409,7 +2519,7 @@
         <v>0.52696245733788394</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2441,7 +2551,7 @@
         <v>0.38303072625698326</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2473,7 +2583,7 @@
         <v>0.43648960739030024</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2505,7 +2615,7 @@
         <v>0.72899857617465591</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2537,7 +2647,7 @@
         <v>0.60176991150442483</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2569,7 +2679,7 @@
         <v>0.29367564182842831</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2601,7 +2711,7 @@
         <v>0.68217665615141954</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2633,7 +2743,7 @@
         <v>0.45864661654135336</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2665,7 +2775,7 @@
         <v>0.76663858466722834</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2697,7 +2807,7 @@
         <v>0.58869565217391306</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2729,7 +2839,7 @@
         <v>0.65306122448979587</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2761,7 +2871,7 @@
         <v>0.29811866859623731</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2793,7 +2903,7 @@
         <v>0.67407407407407405</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2825,7 +2935,7 @@
         <v>0.17011128775834658</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2857,7 +2967,7 @@
         <v>0.53061224489795922</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2889,7 +2999,7 @@
         <v>0.39473684210526316</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -2921,7 +3031,7 @@
         <v>4.9295774647887321E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -2953,7 +3063,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -2985,7 +3095,7 @@
         <v>0.42105263157894735</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3017,7 +3127,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -3050,7 +3160,7 @@
         <v>0.62952619351674421</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -3082,7 +3192,7 @@
         <v>0.23004655742927688</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -3114,7 +3224,7 @@
         <v>0.19310307879134223</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -3146,7 +3256,7 @@
         <v>0.25805987777948958</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -3178,7 +3288,7 @@
         <v>0.25531710133769608</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -3210,7 +3320,7 @@
         <v>0.1090302649205785</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -3242,7 +3352,7 @@
         <v>0.23006125028356614</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -3274,7 +3384,7 @@
         <v>0.2761504617701851</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -3306,7 +3416,7 @@
         <v>0.12953979837178892</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -3338,7 +3448,7 @@
         <v>0.15541350379544547</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -3370,7 +3480,7 @@
         <v>0.38307816277195811</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3402,7 +3512,7 @@
         <v>0.22508960573476702</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -3434,7 +3544,7 @@
         <v>0.59945897204688914</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -3466,7 +3576,7 @@
         <v>0.35485413677666189</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>68</v>
       </c>
@@ -3498,7 +3608,7 @@
         <v>0.36047654139032181</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -3530,7 +3640,7 @@
         <v>0.65759861506120931</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>68</v>
       </c>
@@ -3562,7 +3672,7 @@
         <v>0.5373654211526282</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>68</v>
       </c>
@@ -3594,7 +3704,7 @@
         <v>0.53688657783555416</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>68</v>
       </c>
@@ -3626,7 +3736,7 @@
         <v>0.44747154319835791</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>68</v>
       </c>
@@ -3658,7 +3768,7 @@
         <v>0.35803969218307008</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>68</v>
       </c>
@@ -3690,7 +3800,7 @@
         <v>0.48665141113653698</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>68</v>
       </c>
@@ -3722,7 +3832,7 @@
         <v>0.25136754363115393</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -3754,7 +3864,7 @@
         <v>8.8741322064594022E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>68</v>
       </c>
@@ -3786,7 +3896,7 @@
         <v>0.42689434364994666</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>68</v>
       </c>
@@ -3818,7 +3928,7 @@
         <v>0.44396720031237796</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>68</v>
       </c>
@@ -3850,7 +3960,7 @@
         <v>0.26454615981380913</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>68</v>
       </c>
@@ -3882,7 +3992,7 @@
         <v>0.62339181286549705</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>68</v>
       </c>
@@ -3914,7 +4024,7 @@
         <v>2.2271714922048997E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>68</v>
       </c>
@@ -3946,7 +4056,7 @@
         <v>0.48433734939759038</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>68</v>
       </c>
@@ -3978,7 +4088,7 @@
         <v>5.3571428571428568E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>68</v>
       </c>
@@ -4010,7 +4120,7 @@
         <v>0.11960132890365449</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>68</v>
       </c>
@@ -4042,7 +4152,7 @@
         <v>0.50557620817843862</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>68</v>
       </c>
@@ -4074,7 +4184,7 @@
         <v>0.53617021276595744</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>68</v>
       </c>
@@ -4106,7 +4216,7 @@
         <v>0.30232558139534882</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>68</v>
       </c>
@@ -4138,7 +4248,7 @@
         <v>0.22413793103448276</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>68</v>
       </c>
@@ -4170,7 +4280,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>68</v>
       </c>
@@ -4202,7 +4312,7 @@
         <v>0.46902654867256638</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>68</v>
       </c>
@@ -4234,7 +4344,7 @@
         <v>0.54255319148936165</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>68</v>
       </c>
@@ -4266,7 +4376,7 @@
         <v>0.62365591397849462</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>68</v>
       </c>
@@ -4298,7 +4408,7 @@
         <v>0.29577464788732394</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>68</v>
       </c>
@@ -4330,7 +4440,7 @@
         <v>0.63235294117647056</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>68</v>
       </c>
@@ -4362,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>68</v>
       </c>
@@ -4394,7 +4504,7 @@
         <v>0.17857142857142858</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>68</v>
       </c>
@@ -4426,7 +4536,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>68</v>
       </c>
@@ -4458,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>68</v>
       </c>
@@ -4490,7 +4600,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>68</v>
       </c>
@@ -4522,7 +4632,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>68</v>
       </c>
@@ -4554,7 +4664,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>68</v>
       </c>
@@ -4586,7 +4696,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>68</v>
       </c>
@@ -4618,7 +4728,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>68</v>
       </c>
@@ -4650,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -4683,7 +4793,7 @@
         <v>0.24262839897610713</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -4715,7 +4825,7 @@
         <v>0.661746619396958</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>120</v>
       </c>
@@ -4747,7 +4857,7 @@
         <v>0.71898270237341388</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -4779,7 +4889,7 @@
         <v>0.60801892427898974</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -4811,7 +4921,7 @@
         <v>0.63522198370653382</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>120</v>
       </c>
@@ -4843,7 +4953,7 @@
         <v>0.79433311277058327</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>120</v>
       </c>
@@ -4875,7 +4985,7 @@
         <v>0.21287696138492548</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -4907,7 +5017,7 @@
         <v>0.80329076932850518</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>120</v>
       </c>
@@ -4939,7 +5049,7 @@
         <v>0.42326805812985197</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>120</v>
       </c>
@@ -4971,7 +5081,7 @@
         <v>0.38925983591831848</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -5003,7 +5113,7 @@
         <v>0.25926830012510299</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -5035,7 +5145,7 @@
         <v>0.78753122124359143</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -5067,7 +5177,7 @@
         <v>0.14838640275387263</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -5099,7 +5209,7 @@
         <v>0.72691360216604894</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -5131,7 +5241,7 @@
         <v>0.57860663269568124</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>120</v>
       </c>
@@ -5163,7 +5273,7 @@
         <v>0.37507383343177791</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>120</v>
       </c>
@@ -5195,7 +5305,7 @@
         <v>0.88449861022022669</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>120</v>
       </c>
@@ -5227,7 +5337,7 @@
         <v>0.23648106904231625</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>120</v>
       </c>
@@ -5259,7 +5369,7 @@
         <v>0.78530377668308704</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>120</v>
       </c>
@@ -5291,7 +5401,7 @@
         <v>0.43495190105359599</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>120</v>
       </c>
@@ -5323,7 +5433,7 @@
         <v>0.14861955117469736</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>120</v>
       </c>
@@ -5355,7 +5465,7 @@
         <v>0.76747679596544882</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>120</v>
       </c>
@@ -5387,7 +5497,7 @@
         <v>0.62940301921317476</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>120</v>
       </c>
@@ -5419,7 +5529,7 @@
         <v>0.38742393509127787</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>120</v>
       </c>
@@ -5451,7 +5561,7 @@
         <v>0.45984101748807632</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>120</v>
       </c>
@@ -5483,7 +5593,7 @@
         <v>0.77176793056190041</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>120</v>
       </c>
@@ -5515,7 +5625,7 @@
         <v>0.43055736001039369</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>120</v>
       </c>
@@ -5547,7 +5657,7 @@
         <v>0.67283748361730011</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>120</v>
       </c>
@@ -5579,7 +5689,7 @@
         <v>8.9165710539255857E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>120</v>
       </c>
@@ -5611,7 +5721,7 @@
         <v>0.77119124032471209</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>120</v>
       </c>
@@ -5643,7 +5753,7 @@
         <v>0.39772273272073511</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>120</v>
       </c>
@@ -5675,7 +5785,7 @@
         <v>0.26373626373626374</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>120</v>
       </c>
@@ -5707,7 +5817,7 @@
         <v>0.60184193617476978</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>120</v>
       </c>
@@ -5739,7 +5849,7 @@
         <v>0.54630474452554745</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>120</v>
       </c>
@@ -5771,7 +5881,7 @@
         <v>0.30326241134751775</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>120</v>
       </c>
@@ -5803,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>120</v>
       </c>
@@ -5835,7 +5945,7 @@
         <v>0.10723114956736712</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>120</v>
       </c>
@@ -5867,7 +5977,7 @@
         <v>0.37022900763358779</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>120</v>
       </c>
@@ -5899,7 +6009,7 @@
         <v>0.17764227642276423</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>120</v>
       </c>
@@ -5931,7 +6041,7 @@
         <v>0.14518147684605756</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>120</v>
       </c>
@@ -5963,7 +6073,7 @@
         <v>0.93116820164808534</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>120</v>
       </c>
@@ -5995,7 +6105,7 @@
         <v>2.5303110173958882E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>120</v>
       </c>
@@ -6027,7 +6137,7 @@
         <v>0.26385542168674697</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>120</v>
       </c>
@@ -6059,7 +6169,7 @@
         <v>5.4781801299907153E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>120</v>
       </c>
@@ -6091,7 +6201,7 @@
         <v>0.92537313432835822</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>120</v>
       </c>
@@ -6123,7 +6233,7 @@
         <v>0.43774069319640563</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>120</v>
       </c>
@@ -6155,7 +6265,7 @@
         <v>8.0858085808580851E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>120</v>
       </c>
@@ -6187,7 +6297,7 @@
         <v>7.796610169491526E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>120</v>
       </c>
@@ -6219,7 +6329,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>120</v>
       </c>
@@ -6251,7 +6361,7 @@
         <v>0.71942446043165464</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>170</v>
       </c>
@@ -7724,7 +7834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>217</v>
       </c>
@@ -7757,7 +7867,7 @@
         <v>0.25040973187578769</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>218</v>
       </c>
@@ -7789,7 +7899,7 @@
         <v>0.15309341746430671</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>218</v>
       </c>
@@ -7821,7 +7931,7 @@
         <v>0.82862002976823301</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>218</v>
       </c>
@@ -7853,7 +7963,7 @@
         <v>0.13293288064768868</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>218</v>
       </c>
@@ -7885,7 +7995,7 @@
         <v>0.58064516129032262</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>218</v>
       </c>
@@ -7917,7 +8027,7 @@
         <v>0.80930232558139537</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>218</v>
       </c>
@@ -7949,7 +8059,7 @@
         <v>0.43103448275862066</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>218</v>
       </c>
@@ -7981,7 +8091,7 @@
         <v>0.3619047619047619</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>218</v>
       </c>
@@ -8013,7 +8123,7 @@
         <v>0.80540540540540539</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>218</v>
       </c>
@@ -8045,7 +8155,7 @@
         <v>0.78531073446327682</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>218</v>
       </c>
@@ -8077,7 +8187,7 @@
         <v>0.60606060606060608</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>218</v>
       </c>
@@ -8109,7 +8219,7 @@
         <v>0.7068965517241379</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>218</v>
       </c>
@@ -8141,7 +8251,7 @@
         <v>0.55102040816326525</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -8173,7 +8283,7 @@
         <v>0.63414634146341464</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>218</v>
       </c>
@@ -8205,7 +8315,7 @@
         <v>0.45945945945945948</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>218</v>
       </c>
@@ -8237,7 +8347,7 @@
         <v>0.48484848484848486</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>218</v>
       </c>
@@ -8269,7 +8379,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>218</v>
       </c>
@@ -8301,7 +8411,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>218</v>
       </c>
@@ -8333,7 +8443,7 @@
         <v>0.26315789473684209</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>218</v>
       </c>
@@ -8365,7 +8475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>218</v>
       </c>
@@ -8397,7 +8507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>218</v>
       </c>
@@ -8429,7 +8539,7 @@
         <v>0.54545454545454541</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>218</v>
       </c>
@@ -8461,7 +8571,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>218</v>
       </c>
@@ -8493,7 +8603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>242</v>
       </c>
@@ -8526,7 +8636,7 @@
         <v>0.29835082458770612</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>243</v>
       </c>
@@ -8611,8 +8721,16 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
+      <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>